<commit_message>
Atualizações até a data de 13/01/2022.
</commit_message>
<xml_diff>
--- a/dados/cap6.xlsx
+++ b/dados/cap6.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\glossario_stf\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5520208A-5771-4BA2-9C5D-AA8095E016E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7C6256-C7F0-4A68-9700-754EDC98125D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1B3479A7-5E3F-4DCF-999A-B0BE5180553E}"/>
+    <workbookView xWindow="31185" yWindow="1590" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{1B3479A7-5E3F-4DCF-999A-B0BE5180553E}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo_6-1" sheetId="5" r:id="rId1"/>
+    <sheet name="acervo_6-2" sheetId="6" r:id="rId2"/>
+    <sheet name="acervo_6-3" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Código</t>
   </si>
@@ -64,6 +66,126 @@
   </si>
   <si>
     <t>Substituição do Relator, art. 38, II, do RISTF</t>
+  </si>
+  <si>
+    <t>Variável</t>
+  </si>
+  <si>
+    <t>Definição</t>
+  </si>
+  <si>
+    <t>Id Processo</t>
+  </si>
+  <si>
+    <t>Chave numérica única para cada processo.</t>
+  </si>
+  <si>
+    <t>Classe</t>
+  </si>
+  <si>
+    <t>Sigla da classe do processo no STF.</t>
+  </si>
+  <si>
+    <t>Número</t>
+  </si>
+  <si>
+    <t>Número do processo no STF.</t>
+  </si>
+  <si>
+    <t>Nome Ministro (a)</t>
+  </si>
+  <si>
+    <t>Informa para qual Ministro o processo foi distribuído</t>
+  </si>
+  <si>
+    <t>Data Andamento</t>
+  </si>
+  <si>
+    <t>Data em que o processo foi distribuído</t>
+  </si>
+  <si>
+    <t>Qtd Ocorrências Processuais</t>
+  </si>
+  <si>
+    <t>Informa a quantidade de ocorrências em cada andamento processual.</t>
+  </si>
+  <si>
+    <t>Descreve qual andamento foi lançado no ato da distribuição.</t>
+  </si>
+  <si>
+    <t>Classificação STF</t>
+  </si>
+  <si>
+    <t>Recursal ou originária</t>
+  </si>
+  <si>
+    <t>Subgrupo Andamento</t>
+  </si>
+  <si>
+    <t>Informa a qual Subgrupo o andamento pertence.</t>
+  </si>
+  <si>
+    <t>Nome do gráfico e/ou tabela</t>
+  </si>
+  <si>
+    <t>Registrados e Distribuídos</t>
+  </si>
+  <si>
+    <t>Quantitativos geral dos processos registrados à Presidência e distribuídos aos Ministros</t>
+  </si>
+  <si>
+    <t>Registro à Presidência</t>
+  </si>
+  <si>
+    <t>Quantitativo dos processos registrados à Presidência</t>
+  </si>
+  <si>
+    <t>Distribuídos aos Ministros</t>
+  </si>
+  <si>
+    <t>Quantitativo dos processos distribuídos aos Ministros</t>
+  </si>
+  <si>
+    <t>Distribuídos e Registrados à Presidência</t>
+  </si>
+  <si>
+    <t>Gráfico em linha dos processos distribuídos por ano</t>
+  </si>
+  <si>
+    <t>Processos pro classe</t>
+  </si>
+  <si>
+    <t>Gráfico em barra dos processos por classe processual</t>
+  </si>
+  <si>
+    <t>Processos Distribuídos aos Ministros</t>
+  </si>
+  <si>
+    <t>Gráfico em barra da distribuição por ministro</t>
+  </si>
+  <si>
+    <t>Gráfico pizza</t>
+  </si>
+  <si>
+    <t>Distribuição por processo recursal ou originário</t>
+  </si>
+  <si>
+    <t>Processos por ramo do direito</t>
+  </si>
+  <si>
+    <t>Mapa de árvore da distribuição por ramo do direito</t>
+  </si>
+  <si>
+    <t>Processos Distribuídos por órgão origem</t>
+  </si>
+  <si>
+    <t>Tabela dos processos distribuídos aos Ministros por órgão origem</t>
+  </si>
+  <si>
+    <t>Processo Registrados por órgão origem</t>
+  </si>
+  <si>
+    <t>Tabela dos processos registrados à Presidência por órgão origem</t>
   </si>
 </sst>
 </file>
@@ -426,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E262F0C4-1CFA-42B1-86DA-1E3CB60A7526}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -511,4 +633,212 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18617AA-D452-4F9E-A2B3-8E7959965241}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0382B5-2B1D-4AA3-B22B-82C8B1984B0E}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>